<commit_message>
Commit 31 1 2017
</commit_message>
<xml_diff>
--- a/Framework/Database/TestDataDB.xlsx
+++ b/Framework/Database/TestDataDB.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="LoginDetails" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1095" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1179" uniqueCount="223">
   <si>
     <t>Application_Details</t>
   </si>
@@ -319,346 +319,391 @@
     <t>URL/HOST</t>
   </si>
   <si>
+    <t>pin</t>
+  </si>
+  <si>
+    <t>BillGeneration_AccountLevel</t>
+  </si>
+  <si>
+    <t>SIMSwap_Guided_Journey</t>
+  </si>
+  <si>
+    <t>SIMSwap Guided journey</t>
+  </si>
+  <si>
+    <t>SIMSwap_Global_Search</t>
+  </si>
+  <si>
+    <t>SIMSwap Global Search</t>
+  </si>
+  <si>
+    <t>Post-paid guided flow</t>
+  </si>
+  <si>
+    <t>TransferOfService</t>
+  </si>
+  <si>
+    <t>Transfer of Service</t>
+  </si>
+  <si>
+    <t>ConsumerFixedLine_Provision</t>
+  </si>
+  <si>
+    <t>PlanSelection_FL</t>
+  </si>
+  <si>
+    <t>OSM_Login</t>
+  </si>
+  <si>
+    <t>OSM_SearchFL</t>
+  </si>
+  <si>
+    <t>EnterpriseFixedLine_Provision</t>
+  </si>
+  <si>
+    <t>PlanSelection_FL_ENT</t>
+  </si>
+  <si>
+    <t>login into OSM</t>
+  </si>
+  <si>
+    <t>Update the Status</t>
+  </si>
+  <si>
+    <t>ConsumerPostpaid_GuidedJourney</t>
+  </si>
+  <si>
+    <t>SiebleValidation</t>
+  </si>
+  <si>
+    <t>TransferOfOwnership</t>
+  </si>
+  <si>
+    <t>ServicePoint</t>
+  </si>
+  <si>
+    <t>Checking service Point</t>
+  </si>
+  <si>
+    <t>IDP</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>NewAccount</t>
+  </si>
+  <si>
+    <t>NewCustomer</t>
+  </si>
+  <si>
+    <t>DP</t>
+  </si>
+  <si>
+    <t>Prepaid_To_Postpaid</t>
+  </si>
+  <si>
+    <t>ConsumerPostpaid</t>
+  </si>
+  <si>
+    <t>ExtCustomer</t>
+  </si>
+  <si>
+    <t>CRM_Level</t>
+  </si>
+  <si>
+    <t>TT</t>
+  </si>
+  <si>
+    <t>Postpaid_To_Prepaid</t>
+  </si>
+  <si>
+    <t>EnterprisePostpaid</t>
+  </si>
+  <si>
+    <t>UpgradePromotion_Account360</t>
+  </si>
+  <si>
+    <t>Upgrading promotion via Account 360</t>
+  </si>
+  <si>
+    <t>Chrome</t>
+  </si>
+  <si>
+    <t>Account360view</t>
+  </si>
+  <si>
+    <t>Account360</t>
+  </si>
+  <si>
+    <t>Account 360 view</t>
+  </si>
+  <si>
+    <t>OpenUI_AccesRrights_6Segments</t>
+  </si>
+  <si>
+    <t>OrderSubmission</t>
+  </si>
+  <si>
+    <t>Order Submition</t>
+  </si>
+  <si>
+    <t>OrderPayments</t>
+  </si>
+  <si>
+    <t>Order level payment</t>
+  </si>
+  <si>
+    <t>ConsumerPrepaid_Provision</t>
+  </si>
+  <si>
+    <t>ConsumerPostpaid_Provision</t>
+  </si>
+  <si>
+    <t>EnterprisePostpaid_Provision</t>
+  </si>
+  <si>
+    <t>EnterprisePrepaid_Provision</t>
+  </si>
+  <si>
+    <t>LocalCall</t>
+  </si>
+  <si>
+    <t>LocalCall_OnNet</t>
+  </si>
+  <si>
+    <t>PrevCheckBalance</t>
+  </si>
+  <si>
+    <t>Pre Balance Check</t>
+  </si>
+  <si>
+    <t>SetCapabilities</t>
+  </si>
+  <si>
+    <t>Setting Mobile Capabilities</t>
+  </si>
+  <si>
+    <t>Making Local Call</t>
+  </si>
+  <si>
+    <t>PostCheckBalance</t>
+  </si>
+  <si>
+    <t>Post Balance Check</t>
+  </si>
+  <si>
+    <t>LocalCallCharging</t>
+  </si>
+  <si>
+    <t>Local Cal Charging Verification</t>
+  </si>
+  <si>
+    <t>InvoiceToPDF_Generation</t>
+  </si>
+  <si>
+    <t>Invoicegeneration</t>
+  </si>
+  <si>
+    <t>Plan selection &amp; order submition</t>
+  </si>
+  <si>
+    <t>MSISDN--97478152661||New_SIM--8962702800901163662||</t>
+  </si>
+  <si>
+    <t>MSISDN--97478152661||New_PlanName--Prepaid Red Promotion||</t>
+  </si>
+  <si>
+    <t>MSISDN--97478152664||New_PlanName--Postpaid Standard Promotion||</t>
+  </si>
+  <si>
+    <t>MSISDN--97478152664||New_PlanName--Prepaid Red Promotion||</t>
+  </si>
+  <si>
+    <t>MSISDN--97478152665||SIM--8962702800901163665||PlanName--Postpaid Red 250 Promotion||</t>
+  </si>
+  <si>
+    <t>PlanDiscount</t>
+  </si>
+  <si>
+    <t>MSISDN--97478152665||New_SIM--8962702800901163666||</t>
+  </si>
+  <si>
+    <t>SingleAccount</t>
+  </si>
+  <si>
+    <t>Brmsitenv@123</t>
+  </si>
+  <si>
+    <t>MSISDN--97478152661||SL_LimitAmount--450||</t>
+  </si>
+  <si>
+    <t>MSISDN--97478152661||</t>
+  </si>
+  <si>
+    <t>MSISDN--97478152661||Add_Addon--Paid Addons,Vodafone Passport||</t>
+  </si>
+  <si>
+    <t>MSISDN--97478152665||New_PlanName--Postpaid Red 350 Promotion||</t>
+  </si>
+  <si>
+    <t>AccountNo--Fetch#IDP||PVT_Date--020112002018||</t>
+  </si>
+  <si>
+    <t>GlobalSearchMSISDN</t>
+  </si>
+  <si>
+    <t>Segment--Royal||Royal_MSISDN--97470899087||Black_MSISDN--97489755046||VVIP_MSISDN--97489756692,97478151045||Qatari_MSISDN--97478152922||Expatriate_MSISDN--97478151043||</t>
+  </si>
+  <si>
+    <t>GlobalSearchContact</t>
+  </si>
+  <si>
+    <t>Segment--Royal||Royal_ContactID--GTYH1234||Black_ContactID--99900007765||VVIP_ContactID--99987876U,23457||Qatari_ContactID--VQFT12370897||Expatriate_ContactID--454345||</t>
+  </si>
+  <si>
+    <t>AssertMSISDNQuery</t>
+  </si>
+  <si>
+    <t>GuidedSIMSwap</t>
+  </si>
+  <si>
+    <t>AccountNameQuery</t>
+  </si>
+  <si>
+    <t>Segment--Royal||Royal_AccountName--VFQA Test OUI SP2 Mav test Live SIM||Black_AccountName--VFQATEST_ EV11_TEST||VVIP_AccountName--VFQATEST_EODS_RetroPost VFQATEST_EODS_RetroPost,VFQATEST_Retest_Ankur VFQATEST_Retest_Ankur||Qatari_AccountName--VFQA_Mav VFQA_Test944||Expatriate_AccountName--VFQATEST_XR188_DataPlan200_Iv VFQATEST_XR188_DataPlan200_Iv||</t>
+  </si>
+  <si>
+    <t>AccountNumberQuery</t>
+  </si>
+  <si>
+    <t>Segment--Royal||Royal_AccountNumber--8959436734||Black_AccountNumber--5637448925||VVIP_AccountNumber--7321895097,7779562981||Qatari_AccountNumber--9811140835||Expatriate_AccountNumber--7769191001||</t>
+  </si>
+  <si>
+    <t>ContactIDQuery</t>
+  </si>
+  <si>
+    <t>Segment--Royal||Royal_MSISDN--97470899087||Black_MSISDN--97489755046||VVIP_MSISDN--97489756692||VIP_MSISDN--97478151045||Qatari_MSISDN--97478152922||Expatriate_MSISDN--97478151043||</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>MSISDN--97478152668||SIM--8962702800901163668||PlanName--Prepaid Red Promotion||</t>
+  </si>
+  <si>
+    <t>MSISDN--97478152668||New_PlanName--Postpaid Red 250 Promotion||</t>
+  </si>
+  <si>
+    <t>MSISDN--97478152668||</t>
+  </si>
+  <si>
+    <t>MSISDN--97478152669||SIM--8962702800901163669||PlanName--Prepaid Red Promotion||</t>
+  </si>
+  <si>
+    <t>MSISDN--97478152669||NEW_MSISDN--97478152662||</t>
+  </si>
+  <si>
+    <t>ConsumerPostpaid_Prov_OrdPay</t>
+  </si>
+  <si>
+    <t>EnterprisePostpaid_Prov_OrdPay</t>
+  </si>
+  <si>
+    <t>MSISDN--97478119570||SIM--8962702800901129570||PlanName--Postpaid Red 350 Promotion||PayType--Cash||PaymentReference--2131234||TransactionAmt--100||</t>
+  </si>
+  <si>
+    <t>AccountNo--10077053778||PVT_Date--020112002018||</t>
+  </si>
+  <si>
+    <t>MSISDN--97478152661||SIM--8962702800901163661||PlanName--Postpaid Red 250 Promotion||Account_No--10092270788||</t>
+  </si>
+  <si>
+    <t>MSISDN--97478152661||PlanName--Postpaid Red 250 Promotion||Discounts--30% Monthly Discount||PlanBundle--Red 250||</t>
+  </si>
+  <si>
+    <t>EnterprisePrepaid</t>
+  </si>
+  <si>
+    <t>MSISDN--97478152662||New_PlanName--Postpaid Standard Promotion||</t>
+  </si>
+  <si>
+    <t>MSISDN--97478152665||</t>
+  </si>
+  <si>
+    <t>MSISDN--97478152665||Pay_Type--Upfront||Channel--Cash||BillAmt--100||Reference--123098763||</t>
+  </si>
+  <si>
+    <t>MSISDN--97478127832||</t>
+  </si>
+  <si>
+    <t>MSISDN--97478127832||New_PlanName--Postpaid Red 350 Promotion||</t>
+  </si>
+  <si>
+    <t>MSISDN--97478152664||SIM--8962702800901163664||PlanName--Postpaid Basic Promotion||Account_No--10109137161||</t>
+  </si>
+  <si>
+    <t>AccountNo--10109137161||</t>
+  </si>
+  <si>
+    <t>AccountNo--10111455142||</t>
+  </si>
+  <si>
     <t>10.162.53.120</t>
   </si>
   <si>
-    <t>pin</t>
-  </si>
-  <si>
-    <t>BillGeneration_AccountLevel</t>
-  </si>
-  <si>
-    <t>SIMSwap_Guided_Journey</t>
-  </si>
-  <si>
-    <t>SIMSwap Guided journey</t>
-  </si>
-  <si>
-    <t>SIMSwap_Global_Search</t>
-  </si>
-  <si>
-    <t>SIMSwap Global Search</t>
-  </si>
-  <si>
-    <t>Post-paid guided flow</t>
-  </si>
-  <si>
-    <t>TransferOfService</t>
-  </si>
-  <si>
-    <t>Transfer of Service</t>
-  </si>
-  <si>
-    <t>ConsumerFixedLine_Provision</t>
-  </si>
-  <si>
-    <t>PlanSelection_FL</t>
-  </si>
-  <si>
-    <t>OSM_Login</t>
-  </si>
-  <si>
-    <t>OSM_SearchFL</t>
-  </si>
-  <si>
-    <t>EnterpriseFixedLine_Provision</t>
-  </si>
-  <si>
-    <t>PlanSelection_FL_ENT</t>
-  </si>
-  <si>
-    <t>login into OSM</t>
-  </si>
-  <si>
-    <t>Update the Status</t>
-  </si>
-  <si>
-    <t>ConsumerPostpaid_GuidedJourney</t>
-  </si>
-  <si>
-    <t>SiebleValidation</t>
-  </si>
-  <si>
-    <t>TransferOfOwnership</t>
-  </si>
-  <si>
-    <t>ServicePoint</t>
-  </si>
-  <si>
-    <t>Checking service Point</t>
-  </si>
-  <si>
-    <t>IDP</t>
-  </si>
-  <si>
-    <t>YES</t>
-  </si>
-  <si>
-    <t>NewAccount</t>
-  </si>
-  <si>
-    <t>NewCustomer</t>
-  </si>
-  <si>
-    <t>DP</t>
-  </si>
-  <si>
-    <t>Prepaid_To_Postpaid</t>
-  </si>
-  <si>
-    <t>ConsumerPostpaid</t>
-  </si>
-  <si>
-    <t>ExtCustomer</t>
-  </si>
-  <si>
-    <t>CRM_Level</t>
-  </si>
-  <si>
-    <t>TT</t>
-  </si>
-  <si>
-    <t>Postpaid_To_Prepaid</t>
-  </si>
-  <si>
-    <t>EnterprisePostpaid</t>
-  </si>
-  <si>
-    <t>UpgradePromotion_Account360</t>
-  </si>
-  <si>
-    <t>Upgrading promotion via Account 360</t>
-  </si>
-  <si>
-    <t>Chrome</t>
-  </si>
-  <si>
-    <t>Account360view</t>
-  </si>
-  <si>
-    <t>Account360</t>
-  </si>
-  <si>
-    <t>Account 360 view</t>
-  </si>
-  <si>
-    <t>OpenUI_AccesRrights_6Segments</t>
-  </si>
-  <si>
-    <t>OrderSubmission</t>
-  </si>
-  <si>
-    <t>Order Submition</t>
-  </si>
-  <si>
-    <t>OrderPayments</t>
-  </si>
-  <si>
-    <t>Order level payment</t>
-  </si>
-  <si>
-    <t>ConsumerPrepaid_Provision</t>
-  </si>
-  <si>
-    <t>ConsumerPostpaid_Provision</t>
-  </si>
-  <si>
-    <t>EnterprisePostpaid_Provision</t>
-  </si>
-  <si>
-    <t>EnterprisePrepaid_Provision</t>
-  </si>
-  <si>
-    <t>LocalCall</t>
-  </si>
-  <si>
-    <t>LocalCall_OnNet</t>
-  </si>
-  <si>
-    <t>PrevCheckBalance</t>
-  </si>
-  <si>
-    <t>Pre Balance Check</t>
-  </si>
-  <si>
-    <t>SetCapabilities</t>
-  </si>
-  <si>
-    <t>Setting Mobile Capabilities</t>
-  </si>
-  <si>
-    <t>Making Local Call</t>
-  </si>
-  <si>
-    <t>PostCheckBalance</t>
-  </si>
-  <si>
-    <t>Post Balance Check</t>
-  </si>
-  <si>
-    <t>LocalCallCharging</t>
-  </si>
-  <si>
-    <t>Local Cal Charging Verification</t>
-  </si>
-  <si>
-    <t>KALISARAVANAN</t>
-  </si>
-  <si>
-    <t>InvoiceToPDF_Generation</t>
-  </si>
-  <si>
-    <t>Invoicegeneration</t>
-  </si>
-  <si>
-    <t>Plan selection &amp; order submition</t>
-  </si>
-  <si>
-    <t>MSISDN--97478152661||New_SIM--8962702800901163662||</t>
-  </si>
-  <si>
-    <t>MSISDN--97478152661||New_PlanName--Prepaid Red Promotion||</t>
-  </si>
-  <si>
-    <t>MSISDN--97478152664||New_PlanName--Postpaid Standard Promotion||</t>
-  </si>
-  <si>
-    <t>MSISDN--97478152664||New_PlanName--Prepaid Red Promotion||</t>
-  </si>
-  <si>
-    <t>MSISDN--97478152665||SIM--8962702800901163665||PlanName--Postpaid Red 250 Promotion||</t>
-  </si>
-  <si>
-    <t>PlanDiscount</t>
-  </si>
-  <si>
-    <t>MSISDN--97478152665||New_SIM--8962702800901163666||</t>
-  </si>
-  <si>
-    <t>SingleAccount</t>
-  </si>
-  <si>
-    <t>Brmsitenv@123</t>
-  </si>
-  <si>
-    <t>MSISDN--97478152661||SL_LimitAmount--450||</t>
-  </si>
-  <si>
-    <t>MSISDN--97478152661||</t>
-  </si>
-  <si>
-    <t>MSISDN--97478152661||Add_Addon--Paid Addons,Vodafone Passport||</t>
-  </si>
-  <si>
-    <t>MSISDN--97478152665||New_PlanName--Postpaid Red 350 Promotion||</t>
-  </si>
-  <si>
-    <t>AccountNo--Fetch#IDP||PVT_Date--020112002018||</t>
-  </si>
-  <si>
-    <t>GlobalSearchMSISDN</t>
-  </si>
-  <si>
-    <t>Segment--Royal||Royal_MSISDN--97470899087||Black_MSISDN--97489755046||VVIP_MSISDN--97489756692,97478151045||Qatari_MSISDN--97478152922||Expatriate_MSISDN--97478151043||</t>
-  </si>
-  <si>
-    <t>GlobalSearchContact</t>
-  </si>
-  <si>
-    <t>Segment--Royal||Royal_ContactID--GTYH1234||Black_ContactID--99900007765||VVIP_ContactID--99987876U,23457||Qatari_ContactID--VQFT12370897||Expatriate_ContactID--454345||</t>
-  </si>
-  <si>
-    <t>AssertMSISDNQuery</t>
-  </si>
-  <si>
-    <t>GuidedSIMSwap</t>
-  </si>
-  <si>
-    <t>AccountNameQuery</t>
-  </si>
-  <si>
-    <t>Segment--Royal||Royal_AccountName--VFQA Test OUI SP2 Mav test Live SIM||Black_AccountName--VFQATEST_ EV11_TEST||VVIP_AccountName--VFQATEST_EODS_RetroPost VFQATEST_EODS_RetroPost,VFQATEST_Retest_Ankur VFQATEST_Retest_Ankur||Qatari_AccountName--VFQA_Mav VFQA_Test944||Expatriate_AccountName--VFQATEST_XR188_DataPlan200_Iv VFQATEST_XR188_DataPlan200_Iv||</t>
-  </si>
-  <si>
-    <t>AccountNumberQuery</t>
-  </si>
-  <si>
-    <t>Segment--Royal||Royal_AccountNumber--8959436734||Black_AccountNumber--5637448925||VVIP_AccountNumber--7321895097,7779562981||Qatari_AccountNumber--9811140835||Expatriate_AccountNumber--7769191001||</t>
-  </si>
-  <si>
-    <t>ContactIDQuery</t>
-  </si>
-  <si>
-    <t>Segment--Royal||Royal_MSISDN--97470899087||Black_MSISDN--97489755046||VVIP_MSISDN--97489756692||VIP_MSISDN--97478151045||Qatari_MSISDN--97478152922||Expatriate_MSISDN--97478151043||</t>
-  </si>
-  <si>
-    <t>NO</t>
-  </si>
-  <si>
-    <t>MSISDN--97478152668||SIM--8962702800901163668||PlanName--Prepaid Red Promotion||</t>
-  </si>
-  <si>
-    <t>MSISDN--97478152668||New_PlanName--Postpaid Red 250 Promotion||</t>
-  </si>
-  <si>
-    <t>MSISDN--97478152668||</t>
-  </si>
-  <si>
-    <t>MSISDN--97478152669||SIM--8962702800901163669||PlanName--Prepaid Red Promotion||</t>
-  </si>
-  <si>
-    <t>MSISDN--97478152669||NEW_MSISDN--97478152662||</t>
-  </si>
-  <si>
-    <t>ConsumerPostpaid_Prov_OrdPay</t>
-  </si>
-  <si>
-    <t>EnterprisePostpaid_Prov_OrdPay</t>
-  </si>
-  <si>
-    <t>MSISDN--97478119570||SIM--8962702800901129570||PlanName--Postpaid Red 350 Promotion||PayType--Cash||PaymentReference--2131234||TransactionAmt--100||</t>
-  </si>
-  <si>
-    <t>AccountNo--10077053778||PVT_Date--020112002018||</t>
-  </si>
-  <si>
-    <t>MSISDN--97478152661||SIM--8962702800901163661||PlanName--Postpaid Red 250 Promotion||Account_No--10092270788||</t>
-  </si>
-  <si>
-    <t>MSISDN--97478152661||PlanName--Postpaid Red 250 Promotion||Discounts--30% Monthly Discount||PlanBundle--Red 250||</t>
-  </si>
-  <si>
-    <t>EnterprisePrepaid</t>
-  </si>
-  <si>
-    <t>MSISDN--97478152662||New_PlanName--Postpaid Standard Promotion||</t>
-  </si>
-  <si>
-    <t>MSISDN--97478152665||</t>
-  </si>
-  <si>
-    <t>MSISDN--97478152665||Pay_Type--Upfront||Channel--Cash||BillAmt--100||Reference--123098763||</t>
-  </si>
-  <si>
-    <t>MSISDN--97478127832||</t>
-  </si>
-  <si>
-    <t>MSISDN--97478127832||New_PlanName--Postpaid Red 350 Promotion||</t>
-  </si>
-  <si>
-    <t>MSISDN--97478152664||SIM--8962702800901163664||PlanName--Postpaid Basic Promotion||Account_No--10109137161||</t>
-  </si>
-  <si>
-    <t>AccountNo--10109137161||</t>
-  </si>
-  <si>
-    <t>AccountNo--10111455142||</t>
-  </si>
-  <si>
-    <t>https://10.162.53.125:4443/ecommunications_oui_enu/start.swe?</t>
-  </si>
-  <si>
-    <t>Mav@2017</t>
+    <t>Production</t>
+  </si>
+  <si>
+    <t>https://10.160.222.20:4443/ecommunications_oui_enu/start.swe?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HaleemBaig </t>
+  </si>
+  <si>
+    <t>Mav@2018</t>
+  </si>
+  <si>
+    <t>MSISDN--97430303030||SIM--8989343489892323||PlanName--Prepaid Red Promotion||</t>
+  </si>
+  <si>
+    <t>ConsumerPrepaid</t>
+  </si>
+  <si>
+    <t>MSISDN--97430303030||New_SIM--47474747747447||</t>
+  </si>
+  <si>
+    <t>MSISDN--97430303030||New_PlanName--Postpaid Red 250 Promotion||</t>
+  </si>
+  <si>
+    <t>MSISDN--97430303030||</t>
+  </si>
+  <si>
+    <t>MSISDN--97422222222||SIM--8989222222222220||PlanName--Postpaid Flex 100 Promotion||</t>
+  </si>
+  <si>
+    <t>MSISDN--97422222222||New_PlanName--Postpaid Flex 200 Promotion||</t>
+  </si>
+  <si>
+    <t>MSISDN--97422222222||NEW_MSISDN--97433333333||</t>
+  </si>
+  <si>
+    <t>MSISDN--97433333333||New_SIM--8989333333333333333||</t>
+  </si>
+  <si>
+    <t>MSISDN--97433333333||Add_Addon--Paid Addons,Vodafone Passport||</t>
+  </si>
+  <si>
+    <t>MSISDN--97444444444||SIM--89894444444444444444||PlanName--Postpaid Red 350 Promotion||</t>
+  </si>
+  <si>
+    <t>AccountNo--Fetch#IDP||</t>
+  </si>
+  <si>
+    <t>MSISDN--97455555555||SIM--8995555555555||PlanName--Postpaid Vodafone Contractor Plan Promotion||</t>
+  </si>
+  <si>
+    <t>DunningProcesss</t>
   </si>
 </sst>
 </file>
@@ -790,7 +835,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -819,6 +864,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1294,8 +1342,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1303,7 +1351,7 @@
     <col min="1" max="1" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="149.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.28515625" bestFit="1" customWidth="1"/>
   </cols>
@@ -1333,19 +1381,19 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>53</v>
+        <v>205</v>
       </c>
       <c r="C2" t="s">
         <v>206</v>
       </c>
       <c r="D2" t="s">
-        <v>155</v>
+        <v>207</v>
       </c>
       <c r="E2" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="F2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1384,18 +1432,18 @@
         <v>92</v>
       </c>
       <c r="C5" t="s">
+        <v>204</v>
+      </c>
+      <c r="D5" t="s">
         <v>94</v>
       </c>
-      <c r="D5" t="s">
-        <v>95</v>
-      </c>
       <c r="E5" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -1407,10 +1455,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D20" sqref="D20:D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1418,10 +1466,10 @@
     <col min="1" max="1" width="6.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="98.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1449,6 +1497,246 @@
       </c>
       <c r="H1" s="10" t="s">
         <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C2" t="s">
+        <v>116</v>
+      </c>
+      <c r="D2" t="s">
+        <v>139</v>
+      </c>
+      <c r="E2" t="s">
+        <v>119</v>
+      </c>
+      <c r="G2" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>117</v>
+      </c>
+      <c r="C3" t="s">
+        <v>120</v>
+      </c>
+      <c r="D3" t="s">
+        <v>96</v>
+      </c>
+      <c r="E3" t="s">
+        <v>210</v>
+      </c>
+      <c r="G3" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>117</v>
+      </c>
+      <c r="C4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D4" t="s">
+        <v>69</v>
+      </c>
+      <c r="E4" t="s">
+        <v>121</v>
+      </c>
+      <c r="G4" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>117</v>
+      </c>
+      <c r="C5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D5" t="s">
+        <v>83</v>
+      </c>
+      <c r="E5" t="s">
+        <v>122</v>
+      </c>
+      <c r="G5" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>117</v>
+      </c>
+      <c r="C6" t="s">
+        <v>116</v>
+      </c>
+      <c r="D6" t="s">
+        <v>140</v>
+      </c>
+      <c r="E6" t="s">
+        <v>119</v>
+      </c>
+      <c r="G6" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>117</v>
+      </c>
+      <c r="C7" t="s">
+        <v>120</v>
+      </c>
+      <c r="D7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" t="s">
+        <v>122</v>
+      </c>
+      <c r="G7" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>117</v>
+      </c>
+      <c r="C8" t="s">
+        <v>120</v>
+      </c>
+      <c r="D8" t="s">
+        <v>67</v>
+      </c>
+      <c r="E8" t="s">
+        <v>122</v>
+      </c>
+      <c r="G8" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>117</v>
+      </c>
+      <c r="C9" t="s">
+        <v>120</v>
+      </c>
+      <c r="D9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" t="s">
+        <v>122</v>
+      </c>
+      <c r="G9" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>117</v>
+      </c>
+      <c r="C10" t="s">
+        <v>120</v>
+      </c>
+      <c r="D10" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" t="s">
+        <v>122</v>
+      </c>
+      <c r="G10" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>117</v>
+      </c>
+      <c r="C11" t="s">
+        <v>116</v>
+      </c>
+      <c r="D11" t="s">
+        <v>111</v>
+      </c>
+      <c r="E11" t="s">
+        <v>119</v>
+      </c>
+      <c r="G11" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>117</v>
+      </c>
+      <c r="C12" t="s">
+        <v>120</v>
+      </c>
+      <c r="D12" t="s">
+        <v>113</v>
+      </c>
+      <c r="E12" t="s">
+        <v>118</v>
+      </c>
+      <c r="G12" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>117</v>
+      </c>
+      <c r="C13" t="s">
+        <v>116</v>
+      </c>
+      <c r="D13" t="s">
+        <v>141</v>
+      </c>
+      <c r="E13" t="s">
+        <v>119</v>
+      </c>
+      <c r="G13" t="s">
+        <v>221</v>
       </c>
     </row>
   </sheetData>
@@ -1460,10 +1748,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:E251"/>
+  <dimension ref="A1:E259"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I169" sqref="I169"/>
+    <sheetView tabSelected="1" topLeftCell="A241" workbookViewId="0">
+      <selection activeCell="E261" sqref="E261"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1496,7 +1784,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>12</v>
@@ -1513,7 +1801,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>14</v>
@@ -1530,7 +1818,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>17</v>
@@ -1547,7 +1835,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>19</v>
@@ -1564,7 +1852,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>21</v>
@@ -1581,7 +1869,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>23</v>
@@ -1598,16 +1886,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C8" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="5" t="s">
         <v>136</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1615,7 +1903,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>25</v>
@@ -1632,7 +1920,7 @@
         <v>1</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>12</v>
@@ -1649,7 +1937,7 @@
         <v>2</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>14</v>
@@ -1666,7 +1954,7 @@
         <v>3</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>17</v>
@@ -1683,7 +1971,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>19</v>
@@ -1700,7 +1988,7 @@
         <v>5</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>21</v>
@@ -1717,7 +2005,7 @@
         <v>6</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>23</v>
@@ -1734,16 +2022,16 @@
         <v>7</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C17" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17" s="5" t="s">
         <v>136</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -1751,7 +2039,7 @@
         <v>8</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>73</v>
@@ -1768,7 +2056,7 @@
         <v>9</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>27</v>
@@ -1785,7 +2073,7 @@
         <v>10</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C20" s="6" t="s">
         <v>29</v>
@@ -1802,7 +2090,7 @@
         <v>11</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C21" s="6" t="s">
         <v>31</v>
@@ -1819,7 +2107,7 @@
         <v>12</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C22" s="6" t="s">
         <v>25</v>
@@ -1836,7 +2124,7 @@
         <v>1</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>12</v>
@@ -1853,7 +2141,7 @@
         <v>2</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>14</v>
@@ -1870,7 +2158,7 @@
         <v>3</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>17</v>
@@ -1887,7 +2175,7 @@
         <v>4</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>19</v>
@@ -1904,7 +2192,7 @@
         <v>5</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>21</v>
@@ -1921,7 +2209,7 @@
         <v>6</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>23</v>
@@ -1938,16 +2226,16 @@
         <v>7</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C30" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E30" s="6" t="s">
         <v>138</v>
-      </c>
-      <c r="D30" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E30" s="6" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -1955,16 +2243,16 @@
         <v>8</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C31" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E31" s="5" t="s">
         <v>136</v>
-      </c>
-      <c r="D31" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E31" s="5" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -1972,7 +2260,7 @@
         <v>9</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C32" s="5" t="s">
         <v>73</v>
@@ -1989,7 +2277,7 @@
         <v>10</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C33" s="6" t="s">
         <v>27</v>
@@ -2006,7 +2294,7 @@
         <v>11</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C34" s="6" t="s">
         <v>29</v>
@@ -2023,7 +2311,7 @@
         <v>12</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C35" s="6" t="s">
         <v>31</v>
@@ -2040,7 +2328,7 @@
         <v>13</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C36" s="6" t="s">
         <v>25</v>
@@ -2448,7 +2736,7 @@
         <v>1</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C65" s="5" t="s">
         <v>12</v>
@@ -2465,7 +2753,7 @@
         <v>2</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C66" s="5" t="s">
         <v>39</v>
@@ -2482,7 +2770,7 @@
         <v>3</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C67" s="5" t="s">
         <v>41</v>
@@ -2499,7 +2787,7 @@
         <v>4</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C68" s="5" t="s">
         <v>19</v>
@@ -2516,7 +2804,7 @@
         <v>5</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C69" s="5" t="s">
         <v>21</v>
@@ -2533,7 +2821,7 @@
         <v>6</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C70" s="5" t="s">
         <v>23</v>
@@ -2550,16 +2838,16 @@
         <v>7</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C71" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="D71" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E71" s="5" t="s">
         <v>136</v>
-      </c>
-      <c r="D71" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E71" s="5" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
@@ -2567,7 +2855,7 @@
         <v>8</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C72" s="5" t="s">
         <v>73</v>
@@ -2584,7 +2872,7 @@
         <v>9</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C73" s="6" t="s">
         <v>27</v>
@@ -2601,7 +2889,7 @@
         <v>10</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C74" s="6" t="s">
         <v>29</v>
@@ -2618,7 +2906,7 @@
         <v>11</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C75" s="6" t="s">
         <v>31</v>
@@ -2635,7 +2923,7 @@
         <v>12</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C76" s="5" t="s">
         <v>25</v>
@@ -2655,7 +2943,7 @@
         <v>1</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C78" s="5" t="s">
         <v>12</v>
@@ -2672,7 +2960,7 @@
         <v>2</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C79" s="5" t="s">
         <v>39</v>
@@ -2689,7 +2977,7 @@
         <v>3</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C80" s="5" t="s">
         <v>41</v>
@@ -2706,7 +2994,7 @@
         <v>4</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C81" s="5" t="s">
         <v>19</v>
@@ -2723,7 +3011,7 @@
         <v>5</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C82" s="5" t="s">
         <v>21</v>
@@ -2740,7 +3028,7 @@
         <v>6</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C83" s="5" t="s">
         <v>23</v>
@@ -2757,16 +3045,16 @@
         <v>7</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C84" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="D84" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E84" s="6" t="s">
         <v>138</v>
-      </c>
-      <c r="D84" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E84" s="6" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
@@ -2774,16 +3062,16 @@
         <v>8</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C85" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="D85" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E85" s="5" t="s">
         <v>136</v>
-      </c>
-      <c r="D85" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E85" s="5" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
@@ -2791,7 +3079,7 @@
         <v>9</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C86" s="5" t="s">
         <v>73</v>
@@ -2808,7 +3096,7 @@
         <v>10</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C87" s="6" t="s">
         <v>27</v>
@@ -2825,7 +3113,7 @@
         <v>11</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C88" s="6" t="s">
         <v>29</v>
@@ -2842,7 +3130,7 @@
         <v>12</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C89" s="6" t="s">
         <v>31</v>
@@ -2859,7 +3147,7 @@
         <v>13</v>
       </c>
       <c r="B90" s="4" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C90" s="5" t="s">
         <v>25</v>
@@ -2879,7 +3167,7 @@
         <v>1</v>
       </c>
       <c r="B92" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C92" s="5" t="s">
         <v>12</v>
@@ -2896,7 +3184,7 @@
         <v>2</v>
       </c>
       <c r="B93" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C93" s="5" t="s">
         <v>39</v>
@@ -2913,7 +3201,7 @@
         <v>3</v>
       </c>
       <c r="B94" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C94" s="5" t="s">
         <v>41</v>
@@ -2930,7 +3218,7 @@
         <v>4</v>
       </c>
       <c r="B95" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C95" s="5" t="s">
         <v>19</v>
@@ -2947,7 +3235,7 @@
         <v>5</v>
       </c>
       <c r="B96" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C96" s="5" t="s">
         <v>21</v>
@@ -2964,7 +3252,7 @@
         <v>6</v>
       </c>
       <c r="B97" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C97" s="5" t="s">
         <v>23</v>
@@ -2981,16 +3269,16 @@
         <v>6</v>
       </c>
       <c r="B98" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C98" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="D98" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E98" s="5" t="s">
         <v>136</v>
-      </c>
-      <c r="D98" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E98" s="5" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
@@ -2998,7 +3286,7 @@
         <v>7</v>
       </c>
       <c r="B99" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C99" s="5" t="s">
         <v>25</v>
@@ -3763,7 +4051,7 @@
         <v>1</v>
       </c>
       <c r="B153" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C153" s="6" t="s">
         <v>90</v>
@@ -3780,10 +4068,10 @@
         <v>2</v>
       </c>
       <c r="B154" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C154" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D154" s="6" t="s">
         <v>15</v>
@@ -3797,7 +4085,7 @@
         <v>3</v>
       </c>
       <c r="B155" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C155" s="6" t="s">
         <v>88</v>
@@ -3814,7 +4102,7 @@
         <v>1</v>
       </c>
       <c r="B157" s="8" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C157" s="6" t="s">
         <v>90</v>
@@ -3831,10 +4119,10 @@
         <v>2</v>
       </c>
       <c r="B158" s="8" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C158" s="6" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D158" s="6" t="s">
         <v>15</v>
@@ -3848,7 +4136,7 @@
         <v>3</v>
       </c>
       <c r="B159" s="8" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C159" s="6" t="s">
         <v>88</v>
@@ -3865,7 +4153,7 @@
         <v>1</v>
       </c>
       <c r="B161" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C161" s="6" t="s">
         <v>12</v>
@@ -3882,16 +4170,16 @@
         <v>2</v>
       </c>
       <c r="B162" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="C162" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="D162" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E162" s="6" t="s">
         <v>97</v>
-      </c>
-      <c r="C162" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="D162" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E162" s="6" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.25">
@@ -3899,7 +4187,7 @@
         <v>3</v>
       </c>
       <c r="B163" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C163" s="6" t="s">
         <v>25</v>
@@ -3923,7 +4211,7 @@
         <v>1</v>
       </c>
       <c r="B165" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C165" s="5" t="s">
         <v>12</v>
@@ -3940,16 +4228,16 @@
         <v>2</v>
       </c>
       <c r="B166" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C166" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D166" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E166" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.25">
@@ -3957,7 +4245,7 @@
         <v>3</v>
       </c>
       <c r="B167" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C167" s="5" t="s">
         <v>73</v>
@@ -3974,7 +4262,7 @@
         <v>4</v>
       </c>
       <c r="B168" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C168" s="5" t="s">
         <v>27</v>
@@ -3991,7 +4279,7 @@
         <v>5</v>
       </c>
       <c r="B169" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C169" s="5" t="s">
         <v>29</v>
@@ -4008,7 +4296,7 @@
         <v>6</v>
       </c>
       <c r="B170" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C170" s="5" t="s">
         <v>31</v>
@@ -4025,7 +4313,7 @@
         <v>9</v>
       </c>
       <c r="B171" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C171" s="5" t="s">
         <v>25</v>
@@ -4042,7 +4330,7 @@
         <v>1</v>
       </c>
       <c r="B173" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C173" s="5" t="s">
         <v>12</v>
@@ -4059,7 +4347,7 @@
         <v>2</v>
       </c>
       <c r="B174" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C174" s="5" t="s">
         <v>27</v>
@@ -4076,7 +4364,7 @@
         <v>3</v>
       </c>
       <c r="B175" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C175" s="6" t="s">
         <v>29</v>
@@ -4093,16 +4381,16 @@
         <v>4</v>
       </c>
       <c r="B176" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="C176" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="D176" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E176" s="6" t="s">
         <v>102</v>
-      </c>
-      <c r="C176" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="D176" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E176" s="6" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.25">
@@ -4110,7 +4398,7 @@
         <v>5</v>
       </c>
       <c r="B177" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C177" s="6" t="s">
         <v>27</v>
@@ -4127,7 +4415,7 @@
         <v>6</v>
       </c>
       <c r="B178" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C178" s="6" t="s">
         <v>79</v>
@@ -4144,7 +4432,7 @@
         <v>7</v>
       </c>
       <c r="B179" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C179" s="5" t="s">
         <v>25</v>
@@ -4263,7 +4551,7 @@
         <v>1</v>
       </c>
       <c r="B189" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C189" s="5" t="s">
         <v>12</v>
@@ -4280,7 +4568,7 @@
         <v>2</v>
       </c>
       <c r="B190" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C190" s="5" t="s">
         <v>14</v>
@@ -4297,16 +4585,16 @@
         <v>3</v>
       </c>
       <c r="B191" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C191" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="D191" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E191" s="5" t="s">
         <v>115</v>
-      </c>
-      <c r="D191" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E191" s="5" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.25">
@@ -4314,7 +4602,7 @@
         <v>4</v>
       </c>
       <c r="B192" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C192" s="5" t="s">
         <v>17</v>
@@ -4331,7 +4619,7 @@
         <v>5</v>
       </c>
       <c r="B193" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C193" s="5" t="s">
         <v>19</v>
@@ -4348,7 +4636,7 @@
         <v>6</v>
       </c>
       <c r="B194" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C194" s="5" t="s">
         <v>21</v>
@@ -4365,16 +4653,16 @@
         <v>7</v>
       </c>
       <c r="B195" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C195" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="C195" s="5" t="s">
-        <v>105</v>
-      </c>
       <c r="D195" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E195" s="5" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.25">
@@ -4382,16 +4670,16 @@
         <v>9</v>
       </c>
       <c r="B196" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C196" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D196" s="6" t="s">
         <v>56</v>
       </c>
       <c r="E196" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.25">
@@ -4399,16 +4687,16 @@
         <v>10</v>
       </c>
       <c r="B197" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C197" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D197" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E197" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.25">
@@ -4416,7 +4704,7 @@
         <v>11</v>
       </c>
       <c r="B198" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C198" s="5" t="s">
         <v>12</v>
@@ -4425,7 +4713,7 @@
         <v>5</v>
       </c>
       <c r="E198" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.25">
@@ -4433,16 +4721,16 @@
         <v>12</v>
       </c>
       <c r="B199" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C199" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D199" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E199" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.25">
@@ -4450,7 +4738,7 @@
         <v>13</v>
       </c>
       <c r="B200" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C200" s="5" t="s">
         <v>25</v>
@@ -4459,7 +4747,7 @@
         <v>5</v>
       </c>
       <c r="E200" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.25">
@@ -4467,7 +4755,7 @@
         <v>1</v>
       </c>
       <c r="B202" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C202" s="5" t="s">
         <v>12</v>
@@ -4484,7 +4772,7 @@
         <v>2</v>
       </c>
       <c r="B203" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C203" s="5" t="s">
         <v>39</v>
@@ -4501,7 +4789,7 @@
         <v>3</v>
       </c>
       <c r="B204" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C204" s="5" t="s">
         <v>41</v>
@@ -4518,7 +4806,7 @@
         <v>4</v>
       </c>
       <c r="B205" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C205" s="5" t="s">
         <v>19</v>
@@ -4535,7 +4823,7 @@
         <v>5</v>
       </c>
       <c r="B206" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C206" s="5" t="s">
         <v>21</v>
@@ -4552,10 +4840,10 @@
         <v>6</v>
       </c>
       <c r="B207" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C207" s="5" t="s">
         <v>108</v>
-      </c>
-      <c r="C207" s="5" t="s">
-        <v>109</v>
       </c>
       <c r="D207" s="6" t="s">
         <v>15</v>
@@ -4569,16 +4857,16 @@
         <v>7</v>
       </c>
       <c r="B208" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C208" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="D208" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E208" s="5" t="s">
         <v>136</v>
-      </c>
-      <c r="D208" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E208" s="5" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.25">
@@ -4586,7 +4874,7 @@
         <v>8</v>
       </c>
       <c r="B209" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C209" s="5" t="s">
         <v>25</v>
@@ -4603,7 +4891,7 @@
         <v>1</v>
       </c>
       <c r="B211" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C211" s="5" t="s">
         <v>12</v>
@@ -4620,16 +4908,16 @@
         <v>2</v>
       </c>
       <c r="B212" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C212" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D212" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E212" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.25">
@@ -4637,7 +4925,7 @@
         <v>3</v>
       </c>
       <c r="B213" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C213" s="5" t="s">
         <v>25</v>
@@ -4654,7 +4942,7 @@
         <v>1</v>
       </c>
       <c r="B215" s="8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C215" s="5" t="s">
         <v>12</v>
@@ -4671,16 +4959,16 @@
         <v>2</v>
       </c>
       <c r="B216" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="C216" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="D216" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E216" s="6" t="s">
         <v>129</v>
-      </c>
-      <c r="C216" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="D216" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E216" s="6" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="217" spans="1:5" x14ac:dyDescent="0.25">
@@ -4688,7 +4976,7 @@
         <v>3</v>
       </c>
       <c r="B217" s="8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C217" s="5" t="s">
         <v>73</v>
@@ -4705,7 +4993,7 @@
         <v>4</v>
       </c>
       <c r="B218" s="8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C218" s="5" t="s">
         <v>27</v>
@@ -4722,7 +5010,7 @@
         <v>5</v>
       </c>
       <c r="B219" s="8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C219" s="5" t="s">
         <v>29</v>
@@ -4739,7 +5027,7 @@
         <v>6</v>
       </c>
       <c r="B220" s="8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C220" s="5" t="s">
         <v>31</v>
@@ -4756,7 +5044,7 @@
         <v>7</v>
       </c>
       <c r="B221" s="8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C221" s="5" t="s">
         <v>25</v>
@@ -4774,7 +5062,7 @@
         <v>1</v>
       </c>
       <c r="B223" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C223" s="5" t="s">
         <v>12</v>
@@ -4791,16 +5079,16 @@
         <v>2</v>
       </c>
       <c r="B224" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="C224" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="C224" s="5" t="s">
+      <c r="D224" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E224" s="6" t="s">
         <v>133</v>
-      </c>
-      <c r="D224" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E224" s="6" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="225" spans="1:5" x14ac:dyDescent="0.25">
@@ -4808,7 +5096,7 @@
         <v>3</v>
       </c>
       <c r="B225" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C225" s="5" t="s">
         <v>25</v>
@@ -4825,7 +5113,7 @@
         <v>1</v>
       </c>
       <c r="B227" s="8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C227" s="5" t="s">
         <v>12</v>
@@ -4842,16 +5130,16 @@
         <v>2</v>
       </c>
       <c r="B228" s="8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C228" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D228" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E228" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="229" spans="1:5" x14ac:dyDescent="0.25">
@@ -4859,7 +5147,7 @@
         <v>3</v>
       </c>
       <c r="B229" s="8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C229" s="5" t="s">
         <v>25</v>
@@ -4978,7 +5266,7 @@
         <v>1</v>
       </c>
       <c r="B239" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C239" s="5" t="s">
         <v>12</v>
@@ -4995,16 +5283,16 @@
         <v>2</v>
       </c>
       <c r="B240" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="C240" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="D240" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E240" s="6" t="s">
         <v>99</v>
-      </c>
-      <c r="C240" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="D240" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E240" s="6" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="241" spans="1:5" x14ac:dyDescent="0.25">
@@ -5012,7 +5300,7 @@
         <v>3</v>
       </c>
       <c r="B241" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C241" s="5" t="s">
         <v>25</v>
@@ -5080,16 +5368,16 @@
         <v>1</v>
       </c>
       <c r="B247" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="C247" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="C247" s="5" t="s">
+      <c r="D247" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E247" s="6" t="s">
         <v>146</v>
-      </c>
-      <c r="D247" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E247" s="6" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="248" spans="1:5" x14ac:dyDescent="0.25">
@@ -5097,16 +5385,16 @@
         <v>2</v>
       </c>
       <c r="B248" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C248" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="D248" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E248" s="6" t="s">
         <v>148</v>
-      </c>
-      <c r="D248" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E248" s="6" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="249" spans="1:5" x14ac:dyDescent="0.25">
@@ -5114,16 +5402,16 @@
         <v>3</v>
       </c>
       <c r="B249" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C249" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D249" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E249" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="250" spans="1:5" x14ac:dyDescent="0.25">
@@ -5131,16 +5419,16 @@
         <v>4</v>
       </c>
       <c r="B250" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C250" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="D250" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E250" s="6" t="s">
         <v>151</v>
-      </c>
-      <c r="D250" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E250" s="6" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="251" spans="1:5" x14ac:dyDescent="0.25">
@@ -5148,16 +5436,118 @@
         <v>5</v>
       </c>
       <c r="B251" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C251" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="D251" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E251" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="D251" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E251" s="6" t="s">
-        <v>154</v>
+    </row>
+    <row r="254" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A254">
+        <v>1</v>
+      </c>
+      <c r="B254" s="13" t="s">
+        <v>222</v>
+      </c>
+      <c r="C254" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="D254" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="E254" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="255" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A255">
+        <v>2</v>
+      </c>
+      <c r="B255" s="13" t="s">
+        <v>222</v>
+      </c>
+      <c r="C255" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="D255" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E255" s="6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="256" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A256">
+        <v>3</v>
+      </c>
+      <c r="B256" s="13" t="s">
+        <v>222</v>
+      </c>
+      <c r="C256" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="D256" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="E256" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="257" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A257">
+        <v>4</v>
+      </c>
+      <c r="B257" s="13" t="s">
+        <v>222</v>
+      </c>
+      <c r="C257" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="D257" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="E257" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="258" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A258">
+        <v>5</v>
+      </c>
+      <c r="B258" s="13" t="s">
+        <v>222</v>
+      </c>
+      <c r="C258" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="D258" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E258" s="6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="259" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A259">
+        <v>6</v>
+      </c>
+      <c r="B259" s="13" t="s">
+        <v>222</v>
+      </c>
+      <c r="C259" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="D259" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="E259" s="6" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -5171,8 +5561,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView topLeftCell="H4" workbookViewId="0">
-      <selection sqref="A1:AB28"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31:XFD31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5218,19 +5608,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -5238,19 +5628,19 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D3" t="s">
         <v>69</v>
       </c>
       <c r="E3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G3" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -5258,19 +5648,19 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D4" t="s">
         <v>57</v>
       </c>
       <c r="E4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G4" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -5278,19 +5668,19 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D5" t="s">
         <v>60</v>
       </c>
       <c r="E5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G5" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -5298,19 +5688,19 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D6" t="s">
         <v>36</v>
       </c>
       <c r="E6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G6" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -5318,19 +5708,19 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G7" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -5338,19 +5728,19 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D8" t="s">
         <v>85</v>
       </c>
       <c r="E8" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="G8" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -5358,19 +5748,19 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D9" t="s">
         <v>80</v>
       </c>
       <c r="E9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G9" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -5378,19 +5768,19 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C10" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D10" t="s">
         <v>32</v>
       </c>
       <c r="E10" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G10" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -5398,19 +5788,19 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E11" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G11" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -5418,19 +5808,19 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C12" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D12" t="s">
         <v>34</v>
       </c>
       <c r="E12" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G12" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -5438,19 +5828,19 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C13" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D13" t="s">
         <v>69</v>
       </c>
       <c r="E13" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G13" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -5458,19 +5848,19 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C14" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D14" t="s">
         <v>83</v>
       </c>
       <c r="E14" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G14" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -5478,19 +5868,19 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C15" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D15" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E15" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G15" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -5498,19 +5888,19 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C16" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D16" t="s">
         <v>67</v>
       </c>
       <c r="E16" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="G16" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -5518,19 +5908,19 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C17" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D17" t="s">
         <v>71</v>
       </c>
       <c r="E17" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G17" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -5538,19 +5928,19 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C18" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D18" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E18" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G18" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -5558,19 +5948,19 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C19" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D19" t="s">
         <v>36</v>
       </c>
       <c r="E19" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G19" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -5578,19 +5968,19 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C20" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D20" t="s">
         <v>71</v>
       </c>
       <c r="E20" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G20" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -5598,19 +5988,19 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C21" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D21" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E21" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G21" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -5618,19 +6008,19 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C22" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D22" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E22" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G22" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -5638,19 +6028,19 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C23" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D23" t="s">
         <v>84</v>
       </c>
       <c r="E23" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G23" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -5658,19 +6048,19 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C24" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D24" t="s">
         <v>81</v>
       </c>
       <c r="E24" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G24" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -5678,19 +6068,19 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C25" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D25" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E25" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G25" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -5698,19 +6088,19 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C26" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D26" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E26" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G26" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -5718,19 +6108,19 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C27" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D27" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E27" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G27" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -5738,19 +6128,19 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C28" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D28" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E28" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="G28" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -5758,19 +6148,19 @@
         <v>1</v>
       </c>
       <c r="B30" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C30" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D30" t="s">
+        <v>189</v>
+      </c>
+      <c r="E30" t="s">
+        <v>119</v>
+      </c>
+      <c r="G30" t="s">
         <v>191</v>
-      </c>
-      <c r="E30" t="s">
-        <v>120</v>
-      </c>
-      <c r="G30" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -5778,19 +6168,19 @@
         <v>27</v>
       </c>
       <c r="B31" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C31" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D31" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E31" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="G31" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
   </sheetData>
@@ -5849,19 +6239,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="G2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -5869,19 +6259,19 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E3" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="G3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -5889,19 +6279,19 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E4" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="G4" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -5909,19 +6299,19 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E5" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="G5" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -5929,19 +6319,19 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E6" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="G6" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -5949,19 +6339,19 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E7" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="G7" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -5969,19 +6359,19 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E8" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="G8" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>

</xml_diff>